<commit_message>
adding movie files, editing the mnovie assignment
</commit_message>
<xml_diff>
--- a/class_materials/projects/movies/tropes.xlsx
+++ b/class_materials/projects/movies/tropes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliobruna/Dropbox (UFL)/Teaching/IDS 2935 - Future of Rain Forests/IDS2935_website/assignments/01_movies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliobruna/Dropbox (UFL)/Teaching/IDS 2935 - Future of Rain Forests/IDS2935_RainForests/class_materials/projects/movies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEBC8FA-74C4-544B-AEA6-8ACC38B87C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E69FF0-15BB-6E44-ADD5-440A3B784D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="36700" windowHeight="16940" xr2:uid="{1796CE39-9A6F-4C48-8928-FB2A8F5D27AA}"/>
+    <workbookView xWindow="-46340" yWindow="4160" windowWidth="36700" windowHeight="16940" xr2:uid="{1796CE39-9A6F-4C48-8928-FB2A8F5D27AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="290">
   <si>
     <t>Action, Plot, Mood, Props</t>
   </si>
@@ -345,9 +345,6 @@
     </r>
   </si>
   <si>
-    <t>Cracking Branch at the worst possible moment</t>
-  </si>
-  <si>
     <t>Deadly Road Trip</t>
   </si>
   <si>
@@ -1229,12 +1226,6 @@
     <t>The usual way of transportation of a Nature Hero: grab a conveniently placed, always available vine on a tree, and swing on it to the next one.</t>
   </si>
   <si>
-    <t>walking through a spiderweb</t>
-  </si>
-  <si>
-    <t>you have a tarantula on you</t>
-  </si>
-  <si>
     <t>Characters</t>
   </si>
   <si>
@@ -5570,8 +5561,20 @@
     <t xml:space="preserve">https://tvtropes.org/pmwiki/pmwiki.php/Main/AppeaseTheVolcanoGod </t>
   </si>
   <si>
-    <r>
-      <t> Beige or tan linens, big brown belt, boots, probably a rifle and binoculars; also, a safari hat called a pith helmet. (</t>
+    <t xml:space="preserve">Maybe it comes out of nowhere. Maybe you're in a heated fight. But no matter the circumstances, that blowdart / bullet / axe / arrow / spear just missed your head and buried itself in the tree next to you. At eye level, so we can see the look on your face. Whew! </t>
+  </si>
+  <si>
+    <t>Or maybe you were running. But sp[iderwebs are icky, giant, sticky fish nets and you just ran through one.</t>
+  </si>
+  <si>
+    <t>Don't. Move. I'm going just going to brush this Tarantula / Scorpion / Giant Centipede off your shoulder….</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This warning - or some variation - will be spoken by the grizzled veteran of jungle adventures to the first-time rain forest visitors.  </t>
+  </si>
+  <si>
+    <r>
+      <t>Beige or tan linens, big brown belt, boots, probably a rifle and binoculars; also, a safari hat called a pith helmet. (</t>
     </r>
     <r>
       <rPr>
@@ -5681,6 +5684,18 @@
       </rPr>
       <t> vintage, not the broad-brimmed "Bombay Bowler" of the post-1900 years.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cracking Branch </t>
+  </si>
+  <si>
+    <t>The moment when absolute sience is required…that's when someone will step on a branch. The noise of the branch breaking - louder than any gunshot - will reveal their position. RUUUUNNNN!!!!!</t>
+  </si>
+  <si>
+    <t>Walking into spiderwebs</t>
+  </si>
+  <si>
+    <t>There's a tarantula on your shoulder</t>
   </si>
 </sst>
 </file>
@@ -6277,8 +6292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5280EC06-5984-9B4C-BD6E-3184906634AE}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6289,16 +6304,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1" t="s">
         <v>279</v>
       </c>
-      <c r="B1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C1" t="s">
-        <v>282</v>
-      </c>
       <c r="D1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6309,7 +6324,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -6326,7 +6341,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6362,22 +6377,24 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>286</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -6385,13 +6402,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -6399,13 +6416,13 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -6413,13 +6430,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -6427,13 +6444,13 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6441,13 +6458,13 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
         <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -6455,13 +6472,13 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -6469,13 +6486,13 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -6483,13 +6500,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
         <v>36</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -6497,13 +6514,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -6511,13 +6528,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -6525,13 +6542,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -6539,13 +6556,13 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -6553,13 +6570,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -6567,13 +6584,13 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -6581,13 +6598,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -6595,13 +6612,13 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -6609,13 +6626,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -6623,13 +6640,13 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
         <v>66</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -6637,22 +6654,24 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>0</v>
       </c>
       <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
         <v>70</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -6660,13 +6679,13 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
         <v>73</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -6674,13 +6693,13 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -6688,932 +6707,939 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>288</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>289</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D47" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D48" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
-      </c>
-      <c r="C53" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D54" t="s">
         <v>145</v>
-      </c>
-      <c r="B54" t="s">
-        <v>147</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D54" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D55" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="D56" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D58" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D64" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D65" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D67" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D68" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D70" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D72" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B73" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D73" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D74" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D76" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D79" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C80" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
+        <v>225</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="D81" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C91" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>